<commit_message>
[Manual] cafe24 쇼핑몰 설정 manual update
</commit_message>
<xml_diff>
--- a/Cafe24_shopping mall Setup manual.xlsx
+++ b/Cafe24_shopping mall Setup manual.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="상점관리" sheetId="1" r:id="rId1"/>
+    <sheet name="기타이용안내설정" sheetId="3" r:id="rId1"/>
+    <sheet name="상점관리" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>배송/반품 설정</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -37,6 +38,34 @@
   </si>
   <si>
     <t>배송에 대한 추가 설명이 필요한 경우 표시할 text 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지역별 배송비 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제주 및 도서지역에 대한 추가 배송비 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상품결제안내 내용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타이용안내 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원가입안내</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배송안내</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>교환안내</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -110,6 +139,432 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="19" name="그룹 18"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="828675" y="485775"/>
+          <a:ext cx="6677025" cy="4762500"/>
+          <a:chOff x="828675" y="485775"/>
+          <a:chExt cx="6677025" cy="4762500"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="18" name="그림 17"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="828675" y="485775"/>
+            <a:ext cx="6677025" cy="4762500"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="8" name="모서리가 둥근 직사각형 7"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="914399" y="2400300"/>
+            <a:ext cx="1704975" cy="304800"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:noFill/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="그림 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1038225" y="4638675"/>
+          <a:ext cx="9353550" cy="1790700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="27" name="그룹 26"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="952500" y="13839825"/>
+          <a:ext cx="9544050" cy="5572125"/>
+          <a:chOff x="952500" y="13839825"/>
+          <a:chExt cx="9544050" cy="5572125"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="21" name="그림 20"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="952500" y="13839825"/>
+            <a:ext cx="9544050" cy="5572125"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="22" name="모서리가 둥근 직사각형 21"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2466975" y="14830425"/>
+            <a:ext cx="809625" cy="304800"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:noFill/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="26" name="그룹 25"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="942975" y="7791450"/>
+          <a:ext cx="9324975" cy="5524500"/>
+          <a:chOff x="942975" y="7791450"/>
+          <a:chExt cx="9324975" cy="5524500"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:pic>
+        <xdr:nvPicPr>
+          <xdr:cNvPr id="24" name="그림 23"/>
+          <xdr:cNvPicPr>
+            <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          </xdr:cNvPicPr>
+        </xdr:nvPicPr>
+        <xdr:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+            <a:extLst>
+              <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+                <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              </a:ext>
+            </a:extLst>
+          </a:blip>
+          <a:srcRect/>
+          <a:stretch>
+            <a:fillRect/>
+          </a:stretch>
+        </xdr:blipFill>
+        <xdr:spPr bwMode="auto">
+          <a:xfrm>
+            <a:off x="942975" y="7791450"/>
+            <a:ext cx="9324975" cy="5524500"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:extLst>
+            <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+              <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+                <a:solidFill>
+                  <a:srgbClr val="FFFFFF"/>
+                </a:solidFill>
+              </a14:hiddenFill>
+            </a:ext>
+          </a:extLst>
+        </xdr:spPr>
+      </xdr:pic>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="25" name="모서리가 둥근 직사각형 24"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2476500" y="8763000"/>
+            <a:ext cx="809625" cy="304800"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+              </a:ln>
+              <a:noFill/>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -329,6 +784,302 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="그림 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="990600" y="15497175"/>
+          <a:ext cx="6029325" cy="2933700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="그림 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="11572875"/>
+          <a:ext cx="9886950" cy="3667125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="모서리가 둥근 직사각형 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2781300" y="5924550"/>
+          <a:ext cx="952500" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:noFill/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="모서리가 둥근 직사각형 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2686050" y="12315825"/>
+          <a:ext cx="952500" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100">
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:noFill/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="직선 화살표 연결선 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2714625" y="13449300"/>
+          <a:ext cx="7477125" cy="1952625"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -621,10 +1372,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C45"/>
+  <dimension ref="B2:C66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="S46" sqref="S46"/>
+      <selection activeCell="X37" sqref="X37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.25" customWidth="1"/>
+    <col min="2" max="2" width="5.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C27" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C37" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C66" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:O78"/>
+  <sheetViews>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -664,6 +1458,21 @@
         <v>3</v>
       </c>
     </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C55" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O78" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>